<commit_message>
Resultados terminados (menos histologia)
</commit_message>
<xml_diff>
--- a/resultados/PCA_factor_loadings_sinDTDniGST.xlsx
+++ b/resultados/PCA_factor_loadings_sinDTDniGST.xlsx
@@ -1,27 +1,27 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
-<workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" mc:Ignorable="x15 xr xr6 xr10">
+<workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
   <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="26529"/>
   <workbookPr defaultThemeVersion="166925"/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
-      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="D:\collf\Documents\GitHub\TFM-Ortiguilla\resultados\graficas\"/>
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="D:\collf\Documents\GitHub\TFM-Ortiguilla\resultados\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="8_{494BA108-19CE-4F42-9217-CA786F6A7789}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{FA8BFBD0-BED5-4544-AFF5-73FF45913278}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="-110" yWindow="-110" windowWidth="19420" windowHeight="10300" activeTab="1"/>
+    <workbookView xWindow="-110" yWindow="-110" windowWidth="19420" windowHeight="10300" activeTab="1" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
   <sheets>
     <sheet name="PCA_factor_loadings_sinDTDniGST" sheetId="1" r:id="rId1"/>
     <sheet name="Formato" sheetId="2" r:id="rId2"/>
   </sheets>
-  <calcPr calcId="0"/>
+  <calcPr calcId="191029"/>
 </workbook>
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="52" uniqueCount="32">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="52" uniqueCount="34">
   <si>
     <t>PC</t>
   </si>
@@ -117,15 +117,21 @@
   </si>
   <si>
     <t>% varianza explicada</t>
+  </si>
+  <si>
+    <t>MDA.pie</t>
+  </si>
+  <si>
+    <t>MDA.tent</t>
   </si>
 </sst>
 </file>
 
 <file path=xl/styles.xml><?xml version="1.0" encoding="utf-8"?>
-<styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:x16r2="http://schemas.microsoft.com/office/spreadsheetml/2015/02/main" mc:Ignorable="x14ac x16r2">
+<styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:x16r2="http://schemas.microsoft.com/office/spreadsheetml/2015/02/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" mc:Ignorable="x14ac x16r2 xr">
   <numFmts count="2">
-    <numFmt numFmtId="170" formatCode="0.000"/>
-    <numFmt numFmtId="171" formatCode="0.0%"/>
+    <numFmt numFmtId="164" formatCode="0.000"/>
+    <numFmt numFmtId="165" formatCode="0.0%"/>
   </numFmts>
   <fonts count="21" x14ac:knownFonts="1">
     <font>
@@ -652,21 +658,20 @@
     <xf numFmtId="0" fontId="1" fillId="31" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
     <xf numFmtId="0" fontId="1" fillId="32" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
   </cellStyleXfs>
-  <cellXfs count="19">
+  <cellXfs count="18">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
-    <xf numFmtId="170" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1"/>
-    <xf numFmtId="170" fontId="16" fillId="0" borderId="0" xfId="0" applyNumberFormat="1" applyFont="1"/>
-    <xf numFmtId="171" fontId="0" fillId="0" borderId="0" xfId="1" applyNumberFormat="1" applyFont="1"/>
-    <xf numFmtId="170" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1" applyFont="1"/>
+    <xf numFmtId="164" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1"/>
+    <xf numFmtId="164" fontId="16" fillId="0" borderId="0" xfId="0" applyNumberFormat="1" applyFont="1"/>
+    <xf numFmtId="165" fontId="0" fillId="0" borderId="0" xfId="1" applyNumberFormat="1" applyFont="1"/>
     <xf numFmtId="0" fontId="18" fillId="0" borderId="10" xfId="0" applyFont="1" applyBorder="1"/>
     <xf numFmtId="0" fontId="19" fillId="0" borderId="10" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center"/>
     </xf>
     <xf numFmtId="0" fontId="18" fillId="0" borderId="0" xfId="0" applyFont="1"/>
-    <xf numFmtId="170" fontId="18" fillId="0" borderId="0" xfId="0" applyNumberFormat="1" applyFont="1" applyAlignment="1">
+    <xf numFmtId="164" fontId="18" fillId="0" borderId="0" xfId="0" applyNumberFormat="1" applyFont="1" applyAlignment="1">
       <alignment horizontal="center"/>
     </xf>
-    <xf numFmtId="171" fontId="18" fillId="0" borderId="0" xfId="1" applyNumberFormat="1" applyFont="1" applyBorder="1" applyAlignment="1">
+    <xf numFmtId="165" fontId="18" fillId="0" borderId="0" xfId="1" applyNumberFormat="1" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center"/>
     </xf>
     <xf numFmtId="9" fontId="18" fillId="0" borderId="0" xfId="1" applyFont="1" applyBorder="1" applyAlignment="1">
@@ -674,21 +679,21 @@
     </xf>
     <xf numFmtId="0" fontId="20" fillId="0" borderId="11" xfId="0" applyFont="1" applyBorder="1"/>
     <xf numFmtId="0" fontId="18" fillId="0" borderId="11" xfId="0" applyFont="1" applyBorder="1"/>
-    <xf numFmtId="170" fontId="19" fillId="0" borderId="0" xfId="0" quotePrefix="1" applyNumberFormat="1" applyFont="1" applyAlignment="1">
+    <xf numFmtId="164" fontId="19" fillId="0" borderId="0" xfId="0" quotePrefix="1" applyNumberFormat="1" applyFont="1" applyAlignment="1">
       <alignment horizontal="center"/>
     </xf>
-    <xf numFmtId="170" fontId="19" fillId="0" borderId="0" xfId="0" applyNumberFormat="1" applyFont="1" applyAlignment="1">
+    <xf numFmtId="164" fontId="19" fillId="0" borderId="0" xfId="0" applyNumberFormat="1" applyFont="1" applyAlignment="1">
       <alignment horizontal="center"/>
     </xf>
     <xf numFmtId="0" fontId="18" fillId="0" borderId="12" xfId="0" applyFont="1" applyBorder="1"/>
-    <xf numFmtId="170" fontId="18" fillId="0" borderId="12" xfId="0" applyNumberFormat="1" applyFont="1" applyBorder="1" applyAlignment="1">
+    <xf numFmtId="164" fontId="18" fillId="0" borderId="12" xfId="0" applyNumberFormat="1" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="164" fontId="18" fillId="0" borderId="12" xfId="0" quotePrefix="1" applyNumberFormat="1" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center"/>
     </xf>
     <xf numFmtId="0" fontId="18" fillId="0" borderId="10" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="170" fontId="18" fillId="0" borderId="12" xfId="0" quotePrefix="1" applyNumberFormat="1" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center"/>
     </xf>
   </cellXfs>
   <cellStyles count="43">
@@ -753,23 +758,23 @@
 <xdr:wsDr xmlns:xdr="http://schemas.openxmlformats.org/drawingml/2006/spreadsheetDrawing" xmlns:a="http://schemas.openxmlformats.org/drawingml/2006/main">
   <xdr:twoCellAnchor editAs="oneCell">
     <xdr:from>
-      <xdr:col>0</xdr:col>
-      <xdr:colOff>411783</xdr:colOff>
-      <xdr:row>18</xdr:row>
-      <xdr:rowOff>171766</xdr:rowOff>
+      <xdr:col>1</xdr:col>
+      <xdr:colOff>134470</xdr:colOff>
+      <xdr:row>20</xdr:row>
+      <xdr:rowOff>44825</xdr:rowOff>
     </xdr:from>
     <xdr:to>
-      <xdr:col>7</xdr:col>
-      <xdr:colOff>128678</xdr:colOff>
-      <xdr:row>40</xdr:row>
-      <xdr:rowOff>49893</xdr:rowOff>
+      <xdr:col>6</xdr:col>
+      <xdr:colOff>556616</xdr:colOff>
+      <xdr:row>38</xdr:row>
+      <xdr:rowOff>27642</xdr:rowOff>
     </xdr:to>
     <xdr:pic>
       <xdr:nvPicPr>
-        <xdr:cNvPr id="3" name="Imagen 2">
+        <xdr:cNvPr id="2" name="Imagen 1">
           <a:extLst>
             <a:ext uri="{FF2B5EF4-FFF2-40B4-BE49-F238E27FC236}">
-              <a16:creationId xmlns:a16="http://schemas.microsoft.com/office/drawing/2014/main" id="{267CC60E-CDB0-BB9D-0569-646E4C4571DD}"/>
+              <a16:creationId xmlns:a16="http://schemas.microsoft.com/office/drawing/2014/main" id="{493FA0B8-60C9-01B2-5126-E36DAD84FE91}"/>
             </a:ext>
           </a:extLst>
         </xdr:cNvPr>
@@ -792,8 +797,8 @@
       </xdr:blipFill>
       <xdr:spPr bwMode="auto">
         <a:xfrm>
-          <a:off x="411783" y="3600766"/>
-          <a:ext cx="4908020" cy="4069127"/>
+          <a:off x="896470" y="3795060"/>
+          <a:ext cx="4097675" cy="3344582"/>
         </a:xfrm>
         <a:prstGeom prst="rect">
           <a:avLst/>
@@ -1111,7 +1116,7 @@
 </file>
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0000-000000000000}">
   <dimension ref="A1:K15"/>
   <sheetViews>
     <sheetView workbookViewId="0">
@@ -1292,10 +1297,10 @@
       <c r="B6" s="1">
         <v>2.9871561768456401E-3</v>
       </c>
-      <c r="C6" s="4">
+      <c r="C6" s="1">
         <v>0.49707317042125798</v>
       </c>
-      <c r="D6" s="4">
+      <c r="D6" s="1">
         <v>0.49703669756299501</v>
       </c>
       <c r="E6" s="1">
@@ -1653,11 +1658,11 @@
 </file>
 
 <file path=xl/worksheets/sheet2.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0100-000000000000}">
   <dimension ref="B1:L27"/>
   <sheetViews>
-    <sheetView showGridLines="0" tabSelected="1" topLeftCell="A11" zoomScale="40" zoomScaleNormal="40" workbookViewId="0">
-      <selection activeCell="M27" sqref="M27"/>
+    <sheetView showGridLines="0" tabSelected="1" topLeftCell="A13" zoomScale="85" zoomScaleNormal="85" workbookViewId="0">
+      <selection activeCell="H20" sqref="H20"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultRowHeight="14.5" x14ac:dyDescent="0.35"/>
@@ -1669,503 +1674,503 @@
   <sheetData>
     <row r="1" spans="2:12" ht="15" thickBot="1" x14ac:dyDescent="0.4"/>
     <row r="2" spans="2:12" x14ac:dyDescent="0.35">
-      <c r="B2" s="5"/>
-      <c r="C2" s="6" t="s">
+      <c r="B2" s="4"/>
+      <c r="C2" s="5" t="s">
         <v>13</v>
       </c>
-      <c r="D2" s="6" t="s">
+      <c r="D2" s="5" t="s">
         <v>15</v>
       </c>
-      <c r="E2" s="6" t="s">
+      <c r="E2" s="5" t="s">
         <v>16</v>
       </c>
-      <c r="F2" s="6" t="s">
+      <c r="F2" s="5" t="s">
         <v>17</v>
       </c>
-      <c r="G2" s="6" t="s">
+      <c r="G2" s="5" t="s">
         <v>18</v>
       </c>
-      <c r="H2" s="6" t="s">
+      <c r="H2" s="5" t="s">
         <v>19</v>
       </c>
-      <c r="I2" s="6" t="s">
+      <c r="I2" s="5" t="s">
         <v>20</v>
       </c>
-      <c r="J2" s="6" t="s">
+      <c r="J2" s="5" t="s">
         <v>21</v>
       </c>
-      <c r="K2" s="6" t="s">
+      <c r="K2" s="5" t="s">
         <v>22</v>
       </c>
-      <c r="L2" s="6" t="s">
+      <c r="L2" s="5" t="s">
         <v>14</v>
       </c>
     </row>
     <row r="3" spans="2:12" x14ac:dyDescent="0.35">
-      <c r="B3" s="7" t="s">
+      <c r="B3" s="6" t="s">
         <v>24</v>
       </c>
-      <c r="C3" s="8">
+      <c r="C3" s="7">
         <v>3.90679508651762</v>
       </c>
-      <c r="D3" s="8">
+      <c r="D3" s="7">
         <v>1.87261577100668</v>
       </c>
-      <c r="E3" s="8">
+      <c r="E3" s="7">
         <v>1.60766459012269</v>
       </c>
-      <c r="F3" s="8">
+      <c r="F3" s="7">
         <v>0.87252344792914904</v>
       </c>
-      <c r="G3" s="8">
+      <c r="G3" s="7">
         <v>0.57623042557703497</v>
       </c>
-      <c r="H3" s="8">
+      <c r="H3" s="7">
         <v>0.48301890397792602</v>
       </c>
-      <c r="I3" s="8">
+      <c r="I3" s="7">
         <v>0.28731939554269398</v>
       </c>
-      <c r="J3" s="8">
+      <c r="J3" s="7">
         <v>0.159937577919464</v>
       </c>
-      <c r="K3" s="8">
+      <c r="K3" s="7">
         <v>0.14504242710910401</v>
       </c>
-      <c r="L3" s="8">
+      <c r="L3" s="7">
         <v>8.8852374297635497E-2</v>
       </c>
     </row>
     <row r="4" spans="2:12" x14ac:dyDescent="0.35">
-      <c r="B4" s="7" t="s">
+      <c r="B4" s="6" t="s">
         <v>31</v>
       </c>
-      <c r="C4" s="9">
+      <c r="C4" s="8">
         <v>0.39067950865176199</v>
       </c>
-      <c r="D4" s="9">
+      <c r="D4" s="8">
         <v>0.18726157710066799</v>
       </c>
-      <c r="E4" s="9">
+      <c r="E4" s="8">
         <v>0.16076645901226899</v>
       </c>
-      <c r="F4" s="9">
+      <c r="F4" s="8">
         <v>8.7252344792914896E-2</v>
       </c>
-      <c r="G4" s="9">
+      <c r="G4" s="8">
         <v>5.7623042557703501E-2</v>
       </c>
-      <c r="H4" s="9">
+      <c r="H4" s="8">
         <v>4.8301890397792598E-2</v>
       </c>
-      <c r="I4" s="9">
+      <c r="I4" s="8">
         <v>2.8731939554269399E-2</v>
       </c>
-      <c r="J4" s="9">
+      <c r="J4" s="8">
         <v>1.5993757791946402E-2</v>
       </c>
-      <c r="K4" s="9">
+      <c r="K4" s="8">
         <v>1.4504242710910401E-2</v>
       </c>
-      <c r="L4" s="9">
+      <c r="L4" s="8">
         <v>8.8852374297635501E-3</v>
       </c>
     </row>
     <row r="5" spans="2:12" x14ac:dyDescent="0.35">
-      <c r="B5" s="7" t="s">
+      <c r="B5" s="6" t="s">
         <v>25</v>
       </c>
-      <c r="C5" s="9">
+      <c r="C5" s="8">
         <v>0.39067950865176199</v>
       </c>
-      <c r="D5" s="9">
+      <c r="D5" s="8">
         <v>0.57794108575242997</v>
       </c>
-      <c r="E5" s="9">
+      <c r="E5" s="8">
         <v>0.73870754476469891</v>
       </c>
-      <c r="F5" s="9">
+      <c r="F5" s="8">
         <v>0.82595988955761379</v>
       </c>
-      <c r="G5" s="9">
+      <c r="G5" s="8">
         <v>0.88358293211531724</v>
       </c>
-      <c r="H5" s="9">
+      <c r="H5" s="8">
         <v>0.93188482251310989</v>
       </c>
-      <c r="I5" s="9">
+      <c r="I5" s="8">
         <v>0.96061676206737934</v>
       </c>
-      <c r="J5" s="9">
+      <c r="J5" s="8">
         <v>0.97661051985932579</v>
       </c>
-      <c r="K5" s="9">
+      <c r="K5" s="8">
         <v>0.99111476257023623</v>
       </c>
-      <c r="L5" s="10">
+      <c r="L5" s="9">
         <v>0.99999999999999978</v>
       </c>
     </row>
     <row r="6" spans="2:12" x14ac:dyDescent="0.35">
-      <c r="B6" s="11"/>
-      <c r="C6" s="12"/>
-      <c r="D6" s="12"/>
-      <c r="E6" s="12"/>
-      <c r="F6" s="12"/>
-      <c r="G6" s="12"/>
-      <c r="H6" s="12"/>
-      <c r="I6" s="12"/>
-      <c r="J6" s="12"/>
-      <c r="K6" s="12"/>
-      <c r="L6" s="12"/>
+      <c r="B6" s="10"/>
+      <c r="C6" s="11"/>
+      <c r="D6" s="11"/>
+      <c r="E6" s="11"/>
+      <c r="F6" s="11"/>
+      <c r="G6" s="11"/>
+      <c r="H6" s="11"/>
+      <c r="I6" s="11"/>
+      <c r="J6" s="11"/>
+      <c r="K6" s="11"/>
+      <c r="L6" s="11"/>
     </row>
     <row r="7" spans="2:12" x14ac:dyDescent="0.35">
-      <c r="B7" s="7" t="s">
+      <c r="B7" s="6" t="s">
         <v>3</v>
       </c>
-      <c r="C7" s="8">
+      <c r="C7" s="7">
         <v>2.9871561768456401E-3</v>
       </c>
-      <c r="D7" s="8">
+      <c r="D7" s="7">
         <v>0.49707317042125798</v>
       </c>
-      <c r="E7" s="8">
+      <c r="E7" s="7">
         <v>0.49703669756299501</v>
       </c>
-      <c r="F7" s="8">
+      <c r="F7" s="7">
         <v>7.22547260508591E-2</v>
       </c>
-      <c r="G7" s="8">
+      <c r="G7" s="7">
         <v>-0.10163256943750699</v>
       </c>
-      <c r="H7" s="8">
+      <c r="H7" s="7">
         <v>-0.18991359683261599</v>
       </c>
-      <c r="I7" s="8">
+      <c r="I7" s="7">
         <v>0.59471112603387299</v>
       </c>
-      <c r="J7" s="8">
+      <c r="J7" s="7">
         <v>-0.129505717666176</v>
       </c>
-      <c r="K7" s="8">
+      <c r="K7" s="7">
         <v>8.7902582399334905E-2</v>
       </c>
-      <c r="L7" s="8">
+      <c r="L7" s="7">
         <v>0.27580218313633698</v>
       </c>
     </row>
     <row r="8" spans="2:12" x14ac:dyDescent="0.35">
-      <c r="B8" s="7" t="s">
+      <c r="B8" s="6" t="s">
         <v>4</v>
       </c>
-      <c r="C8" s="13" t="s">
+      <c r="C8" s="12" t="s">
         <v>27</v>
       </c>
-      <c r="D8" s="8">
+      <c r="D8" s="7">
         <v>-0.16870306014721601</v>
       </c>
-      <c r="E8" s="8">
+      <c r="E8" s="7">
         <v>-6.06847075837951E-2</v>
       </c>
-      <c r="F8" s="8">
+      <c r="F8" s="7">
         <v>-0.1161320089778</v>
       </c>
-      <c r="G8" s="8">
+      <c r="G8" s="7">
         <v>8.9115927416599905E-2</v>
       </c>
-      <c r="H8" s="8">
+      <c r="H8" s="7">
         <v>-0.18625351707993701</v>
       </c>
-      <c r="I8" s="8">
+      <c r="I8" s="7">
         <v>9.5479078281119303E-2</v>
       </c>
-      <c r="J8" s="8">
+      <c r="J8" s="7">
         <v>-0.25308925828261503</v>
       </c>
-      <c r="K8" s="8">
+      <c r="K8" s="7">
         <v>0.76285177249603597</v>
       </c>
-      <c r="L8" s="8">
+      <c r="L8" s="7">
         <v>-0.22434913764216799</v>
       </c>
     </row>
     <row r="9" spans="2:12" x14ac:dyDescent="0.35">
-      <c r="B9" s="7" t="s">
+      <c r="B9" s="6" t="s">
         <v>5</v>
       </c>
-      <c r="C9" s="8">
+      <c r="C9" s="7">
         <v>0.38894687732052202</v>
       </c>
-      <c r="D9" s="8">
+      <c r="D9" s="7">
         <v>-4.0254339465913398E-2</v>
       </c>
-      <c r="E9" s="8">
+      <c r="E9" s="7">
         <v>0.28131232377124099</v>
       </c>
-      <c r="F9" s="8">
+      <c r="F9" s="7">
         <v>-7.4425162297875602E-2</v>
       </c>
-      <c r="G9" s="8">
+      <c r="G9" s="7">
         <v>0.61961437572649303</v>
       </c>
-      <c r="H9" s="8">
+      <c r="H9" s="7">
         <v>-8.8812118638953205E-2</v>
       </c>
-      <c r="I9" s="8">
+      <c r="I9" s="7">
         <v>0.157852961907435</v>
       </c>
-      <c r="J9" s="8">
+      <c r="J9" s="7">
         <v>0.141349850925575</v>
       </c>
-      <c r="K9" s="8">
+      <c r="K9" s="7">
         <v>-0.41238616230221298</v>
       </c>
-      <c r="L9" s="8">
+      <c r="L9" s="7">
         <v>-0.39453128477484001</v>
       </c>
     </row>
     <row r="10" spans="2:12" x14ac:dyDescent="0.35">
-      <c r="B10" s="7" t="s">
+      <c r="B10" s="6" t="s">
         <v>6</v>
       </c>
-      <c r="C10" s="8">
+      <c r="C10" s="7">
         <v>-0.20952332207025201</v>
       </c>
-      <c r="D10" s="14" t="s">
+      <c r="D10" s="13" t="s">
         <v>28</v>
       </c>
-      <c r="E10" s="8">
+      <c r="E10" s="7">
         <v>0.24792616032502299</v>
       </c>
-      <c r="F10" s="8">
+      <c r="F10" s="7">
         <v>-0.233356902434631</v>
       </c>
-      <c r="G10" s="8">
+      <c r="G10" s="7">
         <v>4.73112100119871E-3</v>
       </c>
-      <c r="H10" s="8">
+      <c r="H10" s="7">
         <v>0.26110606258431202</v>
       </c>
-      <c r="I10" s="8">
+      <c r="I10" s="7">
         <v>-0.40716204263369898</v>
       </c>
-      <c r="J10" s="8">
+      <c r="J10" s="7">
         <v>-0.24948922297340601</v>
       </c>
-      <c r="K10" s="8">
+      <c r="K10" s="7">
         <v>0.12286042991518201</v>
       </c>
-      <c r="L10" s="8">
+      <c r="L10" s="7">
         <v>-0.47408273868407702</v>
       </c>
     </row>
     <row r="11" spans="2:12" x14ac:dyDescent="0.35">
-      <c r="B11" s="7" t="s">
+      <c r="B11" s="6" t="s">
         <v>7</v>
       </c>
-      <c r="C11" s="8">
+      <c r="C11" s="7">
         <v>0.43570399114811298</v>
       </c>
-      <c r="D11" s="8">
+      <c r="D11" s="7">
         <v>0.115432108386086</v>
       </c>
-      <c r="E11" s="8">
+      <c r="E11" s="7">
         <v>4.4121470162917396E-3</v>
       </c>
-      <c r="F11" s="8">
+      <c r="F11" s="7">
         <v>1.1377887124997601E-2</v>
       </c>
-      <c r="G11" s="8">
+      <c r="G11" s="7">
         <v>0.25846308958310499</v>
       </c>
-      <c r="H11" s="8">
+      <c r="H11" s="7">
         <v>0.541771279215432</v>
       </c>
-      <c r="I11" s="8">
+      <c r="I11" s="7">
         <v>-0.20239528715737201</v>
       </c>
-      <c r="J11" s="8">
+      <c r="J11" s="7">
         <v>-0.29048427979776498</v>
       </c>
-      <c r="K11" s="8">
+      <c r="K11" s="7">
         <v>-3.7111310769619502E-2</v>
       </c>
-      <c r="L11" s="8">
+      <c r="L11" s="7">
         <v>0.55645937046173799</v>
       </c>
     </row>
     <row r="12" spans="2:12" x14ac:dyDescent="0.35">
-      <c r="B12" s="7" t="s">
+      <c r="B12" s="6" t="s">
         <v>8</v>
       </c>
-      <c r="C12" s="8">
+      <c r="C12" s="7">
         <v>0.40494857133635398</v>
       </c>
-      <c r="D12" s="8">
+      <c r="D12" s="7">
         <v>0.16079854413895101</v>
       </c>
-      <c r="E12" s="8">
+      <c r="E12" s="7">
         <v>-0.16645370849802399</v>
       </c>
-      <c r="F12" s="8">
+      <c r="F12" s="7">
         <v>0.13095852320989099</v>
       </c>
-      <c r="G12" s="8">
+      <c r="G12" s="7">
         <v>-0.37820065677050901</v>
       </c>
-      <c r="H12" s="8">
+      <c r="H12" s="7">
         <v>-0.45196358063194703</v>
       </c>
-      <c r="I12" s="8">
+      <c r="I12" s="7">
         <v>-0.22341518271109001</v>
       </c>
-      <c r="J12" s="8">
+      <c r="J12" s="7">
         <v>-0.44375267860338402</v>
       </c>
-      <c r="K12" s="8">
+      <c r="K12" s="7">
         <v>-0.40665975237541602</v>
       </c>
-      <c r="L12" s="8">
+      <c r="L12" s="7">
         <v>-7.6116739726173194E-2</v>
       </c>
     </row>
     <row r="13" spans="2:12" x14ac:dyDescent="0.35">
-      <c r="B13" s="7" t="s">
-        <v>9</v>
-      </c>
-      <c r="C13" s="8">
+      <c r="B13" s="6" t="s">
+        <v>32</v>
+      </c>
+      <c r="C13" s="7">
         <v>-0.265496029713441</v>
       </c>
-      <c r="D13" s="8">
+      <c r="D13" s="7">
         <v>-0.301716672692733</v>
       </c>
-      <c r="E13" s="8">
+      <c r="E13" s="7">
         <v>0.401278881570862</v>
       </c>
-      <c r="F13" s="8">
+      <c r="F13" s="7">
         <v>-0.36916361214300297</v>
       </c>
-      <c r="G13" s="8">
+      <c r="G13" s="7">
         <v>0.22249705630976799</v>
       </c>
-      <c r="H13" s="8">
+      <c r="H13" s="7">
         <v>-0.43804769605100902</v>
       </c>
-      <c r="I13" s="8">
+      <c r="I13" s="7">
         <v>-0.35130741926417403</v>
       </c>
-      <c r="J13" s="8">
+      <c r="J13" s="7">
         <v>-0.237908562247509</v>
       </c>
-      <c r="K13" s="8">
+      <c r="K13" s="7">
         <v>9.4457852474940903E-4</v>
       </c>
-      <c r="L13" s="8">
+      <c r="L13" s="7">
         <v>0.34606847757194598</v>
       </c>
     </row>
     <row r="14" spans="2:12" x14ac:dyDescent="0.35">
-      <c r="B14" s="7" t="s">
-        <v>10</v>
-      </c>
-      <c r="C14" s="8">
+      <c r="B14" s="6" t="s">
+        <v>33</v>
+      </c>
+      <c r="C14" s="7">
         <v>-0.27478522323466398</v>
       </c>
-      <c r="D14" s="8">
+      <c r="D14" s="7">
         <v>4.7757985170299597E-2</v>
       </c>
-      <c r="E14" s="13" t="s">
+      <c r="E14" s="12" t="s">
         <v>29</v>
       </c>
-      <c r="F14" s="8">
+      <c r="F14" s="7">
         <v>-0.42580293122684498</v>
       </c>
-      <c r="G14" s="8">
+      <c r="G14" s="7">
         <v>0.23478076956501601</v>
       </c>
-      <c r="H14" s="8">
+      <c r="H14" s="7">
         <v>3.5142580480295699E-2</v>
       </c>
-      <c r="I14" s="8">
+      <c r="I14" s="7">
         <v>0.42573902592621099</v>
       </c>
-      <c r="J14" s="8">
+      <c r="J14" s="7">
         <v>-0.46338001703578202</v>
       </c>
-      <c r="K14" s="8">
+      <c r="K14" s="7">
         <v>-0.16400904720624301</v>
       </c>
-      <c r="L14" s="8">
+      <c r="L14" s="7">
         <v>-2.3242346965685699E-2</v>
       </c>
     </row>
     <row r="15" spans="2:12" x14ac:dyDescent="0.35">
-      <c r="B15" s="7" t="s">
+      <c r="B15" s="6" t="s">
         <v>11</v>
       </c>
-      <c r="C15" s="8">
+      <c r="C15" s="7">
         <v>0.290340697214645</v>
       </c>
-      <c r="D15" s="8">
+      <c r="D15" s="7">
         <v>0.27274852745956901</v>
       </c>
-      <c r="E15" s="8">
+      <c r="E15" s="7">
         <v>-0.151608012036415</v>
       </c>
-      <c r="F15" s="13" t="s">
+      <c r="F15" s="12" t="s">
         <v>30</v>
       </c>
-      <c r="G15" s="8">
+      <c r="G15" s="7">
         <v>-0.19497445885291501</v>
       </c>
-      <c r="H15" s="8">
+      <c r="H15" s="7">
         <v>-0.10948380619735699</v>
       </c>
-      <c r="I15" s="8">
+      <c r="I15" s="7">
         <v>-5.4326145475003897E-2</v>
       </c>
-      <c r="J15" s="8">
+      <c r="J15" s="7">
         <v>0.50149312386481903</v>
       </c>
-      <c r="K15" s="8">
+      <c r="K15" s="7">
         <v>-1.14063795932753E-2</v>
       </c>
-      <c r="L15" s="8">
+      <c r="L15" s="7">
         <v>0.16995155434334</v>
       </c>
     </row>
     <row r="16" spans="2:12" ht="15" thickBot="1" x14ac:dyDescent="0.4">
-      <c r="B16" s="15" t="s">
+      <c r="B16" s="14" t="s">
         <v>12</v>
       </c>
-      <c r="C16" s="16">
+      <c r="C16" s="15">
         <v>-0.120021234946193</v>
       </c>
-      <c r="D16" s="16">
+      <c r="D16" s="15">
         <v>0.46026882036129602</v>
       </c>
-      <c r="E16" s="18">
+      <c r="E16" s="16">
         <v>-0.36850871427912801</v>
       </c>
-      <c r="F16" s="16">
+      <c r="F16" s="15">
         <v>0.318692790288856</v>
       </c>
-      <c r="G16" s="16">
+      <c r="G16" s="15">
         <v>0.495281656544861</v>
       </c>
-      <c r="H16" s="16">
+      <c r="H16" s="15">
         <v>-0.387664544135497</v>
       </c>
-      <c r="I16" s="16">
+      <c r="I16" s="15">
         <v>-0.21909766863055699</v>
       </c>
-      <c r="J16" s="16">
+      <c r="J16" s="15">
         <v>0.18120433123247801</v>
       </c>
-      <c r="K16" s="16">
+      <c r="K16" s="15">
         <v>0.177183261713137</v>
       </c>
-      <c r="L16" s="16">
+      <c r="L16" s="15">
         <v>0.169006877687843</v>
       </c>
     </row>
@@ -2177,12 +2182,12 @@
       <c r="D17" s="17"/>
       <c r="E17" s="17"/>
       <c r="F17" s="17"/>
-      <c r="G17" s="5"/>
-      <c r="H17" s="5"/>
-      <c r="I17" s="5"/>
-      <c r="J17" s="5"/>
-      <c r="K17" s="5"/>
-      <c r="L17" s="5"/>
+      <c r="G17" s="4"/>
+      <c r="H17" s="4"/>
+      <c r="I17" s="4"/>
+      <c r="J17" s="4"/>
+      <c r="K17" s="4"/>
+      <c r="L17" s="4"/>
     </row>
     <row r="27" spans="2:12" x14ac:dyDescent="0.35">
       <c r="H27">

</xml_diff>